<commit_message>
Changed to two-layer PCB
</commit_message>
<xml_diff>
--- a/01_Hardware/FlivzNexxy_BOM.xlsx
+++ b/01_Hardware/FlivzNexxy_BOM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
   <si>
     <t xml:space="preserve">xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t xml:space="preserve">C32346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total No of SMD Parts</t>
   </si>
 </sst>
 </file>
@@ -643,9 +646,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>666000</xdr:colOff>
+      <xdr:colOff>665640</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -659,7 +662,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="203760"/>
-          <a:ext cx="1352880" cy="375480"/>
+          <a:ext cx="1352520" cy="375120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -682,7 +685,7 @@
   <dimension ref="A2:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4312,6 +4315,15 @@
       </c>
       <c r="J26" s="10"/>
     </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <f aca="false">SUM(C7:C26)</f>
+        <v>35</v>
+      </c>
+    </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12"/>
       <c r="B35" s="12" t="s">
@@ -4386,7 +4398,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4409,7 +4421,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Slight modifications to two-layer version
</commit_message>
<xml_diff>
--- a/01_Hardware/FlivzNexxy_BOM.xlsx
+++ b/01_Hardware/FlivzNexxy_BOM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="98">
   <si>
     <t xml:space="preserve">xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -137,7 +137,10 @@
     <t xml:space="preserve">Your Instructions / Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">C6,C11,C13,C14 </t>
+    <t xml:space="preserve">C13,C14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FH(Guangdong Fenghua Advanced Tech)</t>
   </si>
   <si>
     <t xml:space="preserve">0402CG120J500NT</t>
@@ -152,9 +155,24 @@
     <t xml:space="preserve">C1547</t>
   </si>
   <si>
+    <t xml:space="preserve">C6,C11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAGEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0402JRNPO9BN220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C106203</t>
+  </si>
+  <si>
     <t xml:space="preserve">C15 </t>
   </si>
   <si>
+    <t xml:space="preserve">Samsung Electro-Mechanics</t>
+  </si>
+  <si>
     <t xml:space="preserve">CL05A475MP5NRNC</t>
   </si>
   <si>
@@ -209,7 +227,10 @@
     <t xml:space="preserve">D1 </t>
   </si>
   <si>
-    <t xml:space="preserve">19-213/Y2C-CQ2R2L/3T(CY)</t>
+    <t xml:space="preserve">Lite-On</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTST-C190KSKT</t>
   </si>
   <si>
     <t xml:space="preserve">0603</t>
@@ -221,6 +242,9 @@
     <t xml:space="preserve">L1 </t>
   </si>
   <si>
+    <t xml:space="preserve">Sunlord</t>
+  </si>
+  <si>
     <t xml:space="preserve">SDCL1005C3N9STDF</t>
   </si>
   <si>
@@ -242,6 +266,9 @@
     <t xml:space="preserve">Q1 </t>
   </si>
   <si>
+    <t xml:space="preserve">Alpha &amp; Omega Semiconductor</t>
+  </si>
+  <si>
     <t xml:space="preserve">AO3401A</t>
   </si>
   <si>
@@ -263,6 +290,9 @@
     <t xml:space="preserve">R1,R2,R4,R8,R9,R14,R15 </t>
   </si>
   <si>
+    <t xml:space="preserve">Royal Ohm</t>
+  </si>
+  <si>
     <t xml:space="preserve">0402WGF1002TCE</t>
   </si>
   <si>
@@ -281,6 +311,9 @@
     <t xml:space="preserve">U1 </t>
   </si>
   <si>
+    <t xml:space="preserve">Texas Instruments</t>
+  </si>
+  <si>
     <t xml:space="preserve">OPT3001DNPR</t>
   </si>
   <si>
@@ -293,7 +326,10 @@
     <t xml:space="preserve">U2 </t>
   </si>
   <si>
-    <t xml:space="preserve">nRF52810-QCAA-R</t>
+    <t xml:space="preserve">Nordic Semiconductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRF52811-QCAA-R</t>
   </si>
   <si>
     <t xml:space="preserve">QFN-32</t>
@@ -317,6 +353,9 @@
     <t xml:space="preserve">U6 </t>
   </si>
   <si>
+    <t xml:space="preserve"> Sensirion AG</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHTC3</t>
   </si>
   <si>
@@ -329,7 +368,10 @@
     <t xml:space="preserve">Y1 </t>
   </si>
   <si>
-    <t xml:space="preserve">7V32000035</t>
+    <t xml:space="preserve">Abracon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABM3B-32.000MHZ-B2-T</t>
   </si>
   <si>
     <t xml:space="preserve">SMD-3225_4P</t>
@@ -339,6 +381,9 @@
   </si>
   <si>
     <t xml:space="preserve">Y2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epson</t>
   </si>
   <si>
     <t xml:space="preserve">Q13FC1350000400</t>
@@ -642,11 +687,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>9360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>665640</xdr:colOff>
+      <xdr:colOff>665280</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
@@ -661,8 +706,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9360" y="203760"/>
-          <a:ext cx="1352520" cy="375120"/>
+          <a:off x="9360" y="204120"/>
+          <a:ext cx="1352160" cy="374760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -685,7 +730,7 @@
   <dimension ref="A2:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -764,21 +809,23 @@
         <v>11</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J7" s="10"/>
     </row>
@@ -787,1375 +834,390 @@
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
         <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E9" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E11" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="E13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="F13" s="8"/>
       <c r="G13" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="E14" s="7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="9" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="E15" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="9" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="J15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="E16" s="7" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="9" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="E17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="8"/>
+        <v>50</v>
+      </c>
+      <c r="F17" s="7"/>
       <c r="G17" s="9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="D18" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="E18" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="9" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="J18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D19" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="E19" s="7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="J19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="E20" s="7" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="J20" s="10"/>
-      <c r="L20" s="0"/>
-      <c r="M20" s="0"/>
-      <c r="N20" s="0"/>
-      <c r="O20" s="0"/>
-      <c r="P20" s="0"/>
-      <c r="Q20" s="0"/>
-      <c r="R20" s="0"/>
-      <c r="S20" s="0"/>
-      <c r="T20" s="0"/>
-      <c r="U20" s="0"/>
-      <c r="V20" s="0"/>
-      <c r="W20" s="0"/>
-      <c r="X20" s="0"/>
-      <c r="Y20" s="0"/>
-      <c r="Z20" s="0"/>
-      <c r="AA20" s="0"/>
-      <c r="AB20" s="0"/>
-      <c r="AC20" s="0"/>
-      <c r="AD20" s="0"/>
-      <c r="AE20" s="0"/>
-      <c r="AF20" s="0"/>
-      <c r="AG20" s="0"/>
-      <c r="AH20" s="0"/>
-      <c r="AI20" s="0"/>
-      <c r="AJ20" s="0"/>
-      <c r="AK20" s="0"/>
-      <c r="AL20" s="0"/>
-      <c r="AM20" s="0"/>
-      <c r="AN20" s="0"/>
-      <c r="AO20" s="0"/>
-      <c r="AP20" s="0"/>
-      <c r="AQ20" s="0"/>
-      <c r="AR20" s="0"/>
-      <c r="AS20" s="0"/>
-      <c r="AT20" s="0"/>
-      <c r="AU20" s="0"/>
-      <c r="AV20" s="0"/>
-      <c r="AW20" s="0"/>
-      <c r="AX20" s="0"/>
-      <c r="AY20" s="0"/>
-      <c r="AZ20" s="0"/>
-      <c r="BA20" s="0"/>
-      <c r="BB20" s="0"/>
-      <c r="BC20" s="0"/>
-      <c r="BD20" s="0"/>
-      <c r="BE20" s="0"/>
-      <c r="BF20" s="0"/>
-      <c r="BG20" s="0"/>
-      <c r="BH20" s="0"/>
-      <c r="BI20" s="0"/>
-      <c r="BJ20" s="0"/>
-      <c r="BK20" s="0"/>
-      <c r="BL20" s="0"/>
-      <c r="BM20" s="0"/>
-      <c r="BN20" s="0"/>
-      <c r="BO20" s="0"/>
-      <c r="BP20" s="0"/>
-      <c r="BQ20" s="0"/>
-      <c r="BR20" s="0"/>
-      <c r="BS20" s="0"/>
-      <c r="BT20" s="0"/>
-      <c r="BU20" s="0"/>
-      <c r="BV20" s="0"/>
-      <c r="BW20" s="0"/>
-      <c r="BX20" s="0"/>
-      <c r="BY20" s="0"/>
-      <c r="BZ20" s="0"/>
-      <c r="CA20" s="0"/>
-      <c r="CB20" s="0"/>
-      <c r="CC20" s="0"/>
-      <c r="CD20" s="0"/>
-      <c r="CE20" s="0"/>
-      <c r="CF20" s="0"/>
-      <c r="CG20" s="0"/>
-      <c r="CH20" s="0"/>
-      <c r="CI20" s="0"/>
-      <c r="CJ20" s="0"/>
-      <c r="CK20" s="0"/>
-      <c r="CL20" s="0"/>
-      <c r="CM20" s="0"/>
-      <c r="CN20" s="0"/>
-      <c r="CO20" s="0"/>
-      <c r="CP20" s="0"/>
-      <c r="CQ20" s="0"/>
-      <c r="CR20" s="0"/>
-      <c r="CS20" s="0"/>
-      <c r="CT20" s="0"/>
-      <c r="CU20" s="0"/>
-      <c r="CV20" s="0"/>
-      <c r="CW20" s="0"/>
-      <c r="CX20" s="0"/>
-      <c r="CY20" s="0"/>
-      <c r="CZ20" s="0"/>
-      <c r="DA20" s="0"/>
-      <c r="DB20" s="0"/>
-      <c r="DC20" s="0"/>
-      <c r="DD20" s="0"/>
-      <c r="DE20" s="0"/>
-      <c r="DF20" s="0"/>
-      <c r="DG20" s="0"/>
-      <c r="DH20" s="0"/>
-      <c r="DI20" s="0"/>
-      <c r="DJ20" s="0"/>
-      <c r="DK20" s="0"/>
-      <c r="DL20" s="0"/>
-      <c r="DM20" s="0"/>
-      <c r="DN20" s="0"/>
-      <c r="DO20" s="0"/>
-      <c r="DP20" s="0"/>
-      <c r="DQ20" s="0"/>
-      <c r="DR20" s="0"/>
-      <c r="DS20" s="0"/>
-      <c r="DT20" s="0"/>
-      <c r="DU20" s="0"/>
-      <c r="DV20" s="0"/>
-      <c r="DW20" s="0"/>
-      <c r="DX20" s="0"/>
-      <c r="DY20" s="0"/>
-      <c r="DZ20" s="0"/>
-      <c r="EA20" s="0"/>
-      <c r="EB20" s="0"/>
-      <c r="EC20" s="0"/>
-      <c r="ED20" s="0"/>
-      <c r="EE20" s="0"/>
-      <c r="EF20" s="0"/>
-      <c r="EG20" s="0"/>
-      <c r="EH20" s="0"/>
-      <c r="EI20" s="0"/>
-      <c r="EJ20" s="0"/>
-      <c r="EK20" s="0"/>
-      <c r="EL20" s="0"/>
-      <c r="EM20" s="0"/>
-      <c r="EN20" s="0"/>
-      <c r="EO20" s="0"/>
-      <c r="EP20" s="0"/>
-      <c r="EQ20" s="0"/>
-      <c r="ER20" s="0"/>
-      <c r="ES20" s="0"/>
-      <c r="ET20" s="0"/>
-      <c r="EU20" s="0"/>
-      <c r="EV20" s="0"/>
-      <c r="EW20" s="0"/>
-      <c r="EX20" s="0"/>
-      <c r="EY20" s="0"/>
-      <c r="EZ20" s="0"/>
-      <c r="FA20" s="0"/>
-      <c r="FB20" s="0"/>
-      <c r="FC20" s="0"/>
-      <c r="FD20" s="0"/>
-      <c r="FE20" s="0"/>
-      <c r="FF20" s="0"/>
-      <c r="FG20" s="0"/>
-      <c r="FH20" s="0"/>
-      <c r="FI20" s="0"/>
-      <c r="FJ20" s="0"/>
-      <c r="FK20" s="0"/>
-      <c r="FL20" s="0"/>
-      <c r="FM20" s="0"/>
-      <c r="FN20" s="0"/>
-      <c r="FO20" s="0"/>
-      <c r="FP20" s="0"/>
-      <c r="FQ20" s="0"/>
-      <c r="FR20" s="0"/>
-      <c r="FS20" s="0"/>
-      <c r="FT20" s="0"/>
-      <c r="FU20" s="0"/>
-      <c r="FV20" s="0"/>
-      <c r="FW20" s="0"/>
-      <c r="FX20" s="0"/>
-      <c r="FY20" s="0"/>
-      <c r="FZ20" s="0"/>
-      <c r="GA20" s="0"/>
-      <c r="GB20" s="0"/>
-      <c r="GC20" s="0"/>
-      <c r="GD20" s="0"/>
-      <c r="GE20" s="0"/>
-      <c r="GF20" s="0"/>
-      <c r="GG20" s="0"/>
-      <c r="GH20" s="0"/>
-      <c r="GI20" s="0"/>
-      <c r="GJ20" s="0"/>
-      <c r="GK20" s="0"/>
-      <c r="GL20" s="0"/>
-      <c r="GM20" s="0"/>
-      <c r="GN20" s="0"/>
-      <c r="GO20" s="0"/>
-      <c r="GP20" s="0"/>
-      <c r="GQ20" s="0"/>
-      <c r="GR20" s="0"/>
-      <c r="GS20" s="0"/>
-      <c r="GT20" s="0"/>
-      <c r="GU20" s="0"/>
-      <c r="GV20" s="0"/>
-      <c r="GW20" s="0"/>
-      <c r="GX20" s="0"/>
-      <c r="GY20" s="0"/>
-      <c r="GZ20" s="0"/>
-      <c r="HA20" s="0"/>
-      <c r="HB20" s="0"/>
-      <c r="HC20" s="0"/>
-      <c r="HD20" s="0"/>
-      <c r="HE20" s="0"/>
-      <c r="HF20" s="0"/>
-      <c r="HG20" s="0"/>
-      <c r="HH20" s="0"/>
-      <c r="HI20" s="0"/>
-      <c r="HJ20" s="0"/>
-      <c r="HK20" s="0"/>
-      <c r="HL20" s="0"/>
-      <c r="HM20" s="0"/>
-      <c r="HN20" s="0"/>
-      <c r="HO20" s="0"/>
-      <c r="HP20" s="0"/>
-      <c r="HQ20" s="0"/>
-      <c r="HR20" s="0"/>
-      <c r="HS20" s="0"/>
-      <c r="HT20" s="0"/>
-      <c r="HU20" s="0"/>
-      <c r="HV20" s="0"/>
-      <c r="HW20" s="0"/>
-      <c r="HX20" s="0"/>
-      <c r="HY20" s="0"/>
-      <c r="HZ20" s="0"/>
-      <c r="IA20" s="0"/>
-      <c r="IB20" s="0"/>
-      <c r="IC20" s="0"/>
-      <c r="ID20" s="0"/>
-      <c r="IE20" s="0"/>
-      <c r="IF20" s="0"/>
-      <c r="IG20" s="0"/>
-      <c r="IH20" s="0"/>
-      <c r="II20" s="0"/>
-      <c r="IJ20" s="0"/>
-      <c r="IK20" s="0"/>
-      <c r="IL20" s="0"/>
-      <c r="IM20" s="0"/>
-      <c r="IN20" s="0"/>
-      <c r="IO20" s="0"/>
-      <c r="IP20" s="0"/>
-      <c r="IQ20" s="0"/>
-      <c r="IR20" s="0"/>
-      <c r="IS20" s="0"/>
-      <c r="IT20" s="0"/>
-      <c r="IU20" s="0"/>
-      <c r="IV20" s="0"/>
-      <c r="IW20" s="0"/>
-      <c r="IX20" s="0"/>
-      <c r="IY20" s="0"/>
-      <c r="IZ20" s="0"/>
-      <c r="JA20" s="0"/>
-      <c r="JB20" s="0"/>
-      <c r="JC20" s="0"/>
-      <c r="JD20" s="0"/>
-      <c r="JE20" s="0"/>
-      <c r="JF20" s="0"/>
-      <c r="JG20" s="0"/>
-      <c r="JH20" s="0"/>
-      <c r="JI20" s="0"/>
-      <c r="JJ20" s="0"/>
-      <c r="JK20" s="0"/>
-      <c r="JL20" s="0"/>
-      <c r="JM20" s="0"/>
-      <c r="JN20" s="0"/>
-      <c r="JO20" s="0"/>
-      <c r="JP20" s="0"/>
-      <c r="JQ20" s="0"/>
-      <c r="JR20" s="0"/>
-      <c r="JS20" s="0"/>
-      <c r="JT20" s="0"/>
-      <c r="JU20" s="0"/>
-      <c r="JV20" s="0"/>
-      <c r="JW20" s="0"/>
-      <c r="JX20" s="0"/>
-      <c r="JY20" s="0"/>
-      <c r="JZ20" s="0"/>
-      <c r="KA20" s="0"/>
-      <c r="KB20" s="0"/>
-      <c r="KC20" s="0"/>
-      <c r="KD20" s="0"/>
-      <c r="KE20" s="0"/>
-      <c r="KF20" s="0"/>
-      <c r="KG20" s="0"/>
-      <c r="KH20" s="0"/>
-      <c r="KI20" s="0"/>
-      <c r="KJ20" s="0"/>
-      <c r="KK20" s="0"/>
-      <c r="KL20" s="0"/>
-      <c r="KM20" s="0"/>
-      <c r="KN20" s="0"/>
-      <c r="KO20" s="0"/>
-      <c r="KP20" s="0"/>
-      <c r="KQ20" s="0"/>
-      <c r="KR20" s="0"/>
-      <c r="KS20" s="0"/>
-      <c r="KT20" s="0"/>
-      <c r="KU20" s="0"/>
-      <c r="KV20" s="0"/>
-      <c r="KW20" s="0"/>
-      <c r="KX20" s="0"/>
-      <c r="KY20" s="0"/>
-      <c r="KZ20" s="0"/>
-      <c r="LA20" s="0"/>
-      <c r="LB20" s="0"/>
-      <c r="LC20" s="0"/>
-      <c r="LD20" s="0"/>
-      <c r="LE20" s="0"/>
-      <c r="LF20" s="0"/>
-      <c r="LG20" s="0"/>
-      <c r="LH20" s="0"/>
-      <c r="LI20" s="0"/>
-      <c r="LJ20" s="0"/>
-      <c r="LK20" s="0"/>
-      <c r="LL20" s="0"/>
-      <c r="LM20" s="0"/>
-      <c r="LN20" s="0"/>
-      <c r="LO20" s="0"/>
-      <c r="LP20" s="0"/>
-      <c r="LQ20" s="0"/>
-      <c r="LR20" s="0"/>
-      <c r="LS20" s="0"/>
-      <c r="LT20" s="0"/>
-      <c r="LU20" s="0"/>
-      <c r="LV20" s="0"/>
-      <c r="LW20" s="0"/>
-      <c r="LX20" s="0"/>
-      <c r="LY20" s="0"/>
-      <c r="LZ20" s="0"/>
-      <c r="MA20" s="0"/>
-      <c r="MB20" s="0"/>
-      <c r="MC20" s="0"/>
-      <c r="MD20" s="0"/>
-      <c r="ME20" s="0"/>
-      <c r="MF20" s="0"/>
-      <c r="MG20" s="0"/>
-      <c r="MH20" s="0"/>
-      <c r="MI20" s="0"/>
-      <c r="MJ20" s="0"/>
-      <c r="MK20" s="0"/>
-      <c r="ML20" s="0"/>
-      <c r="MM20" s="0"/>
-      <c r="MN20" s="0"/>
-      <c r="MO20" s="0"/>
-      <c r="MP20" s="0"/>
-      <c r="MQ20" s="0"/>
-      <c r="MR20" s="0"/>
-      <c r="MS20" s="0"/>
-      <c r="MT20" s="0"/>
-      <c r="MU20" s="0"/>
-      <c r="MV20" s="0"/>
-      <c r="MW20" s="0"/>
-      <c r="MX20" s="0"/>
-      <c r="MY20" s="0"/>
-      <c r="MZ20" s="0"/>
-      <c r="NA20" s="0"/>
-      <c r="NB20" s="0"/>
-      <c r="NC20" s="0"/>
-      <c r="ND20" s="0"/>
-      <c r="NE20" s="0"/>
-      <c r="NF20" s="0"/>
-      <c r="NG20" s="0"/>
-      <c r="NH20" s="0"/>
-      <c r="NI20" s="0"/>
-      <c r="NJ20" s="0"/>
-      <c r="NK20" s="0"/>
-      <c r="NL20" s="0"/>
-      <c r="NM20" s="0"/>
-      <c r="NN20" s="0"/>
-      <c r="NO20" s="0"/>
-      <c r="NP20" s="0"/>
-      <c r="NQ20" s="0"/>
-      <c r="NR20" s="0"/>
-      <c r="NS20" s="0"/>
-      <c r="NT20" s="0"/>
-      <c r="NU20" s="0"/>
-      <c r="NV20" s="0"/>
-      <c r="NW20" s="0"/>
-      <c r="NX20" s="0"/>
-      <c r="NY20" s="0"/>
-      <c r="NZ20" s="0"/>
-      <c r="OA20" s="0"/>
-      <c r="OB20" s="0"/>
-      <c r="OC20" s="0"/>
-      <c r="OD20" s="0"/>
-      <c r="OE20" s="0"/>
-      <c r="OF20" s="0"/>
-      <c r="OG20" s="0"/>
-      <c r="OH20" s="0"/>
-      <c r="OI20" s="0"/>
-      <c r="OJ20" s="0"/>
-      <c r="OK20" s="0"/>
-      <c r="OL20" s="0"/>
-      <c r="OM20" s="0"/>
-      <c r="ON20" s="0"/>
-      <c r="OO20" s="0"/>
-      <c r="OP20" s="0"/>
-      <c r="OQ20" s="0"/>
-      <c r="OR20" s="0"/>
-      <c r="OS20" s="0"/>
-      <c r="OT20" s="0"/>
-      <c r="OU20" s="0"/>
-      <c r="OV20" s="0"/>
-      <c r="OW20" s="0"/>
-      <c r="OX20" s="0"/>
-      <c r="OY20" s="0"/>
-      <c r="OZ20" s="0"/>
-      <c r="PA20" s="0"/>
-      <c r="PB20" s="0"/>
-      <c r="PC20" s="0"/>
-      <c r="PD20" s="0"/>
-      <c r="PE20" s="0"/>
-      <c r="PF20" s="0"/>
-      <c r="PG20" s="0"/>
-      <c r="PH20" s="0"/>
-      <c r="PI20" s="0"/>
-      <c r="PJ20" s="0"/>
-      <c r="PK20" s="0"/>
-      <c r="PL20" s="0"/>
-      <c r="PM20" s="0"/>
-      <c r="PN20" s="0"/>
-      <c r="PO20" s="0"/>
-      <c r="PP20" s="0"/>
-      <c r="PQ20" s="0"/>
-      <c r="PR20" s="0"/>
-      <c r="PS20" s="0"/>
-      <c r="PT20" s="0"/>
-      <c r="PU20" s="0"/>
-      <c r="PV20" s="0"/>
-      <c r="PW20" s="0"/>
-      <c r="PX20" s="0"/>
-      <c r="PY20" s="0"/>
-      <c r="PZ20" s="0"/>
-      <c r="QA20" s="0"/>
-      <c r="QB20" s="0"/>
-      <c r="QC20" s="0"/>
-      <c r="QD20" s="0"/>
-      <c r="QE20" s="0"/>
-      <c r="QF20" s="0"/>
-      <c r="QG20" s="0"/>
-      <c r="QH20" s="0"/>
-      <c r="QI20" s="0"/>
-      <c r="QJ20" s="0"/>
-      <c r="QK20" s="0"/>
-      <c r="QL20" s="0"/>
-      <c r="QM20" s="0"/>
-      <c r="QN20" s="0"/>
-      <c r="QO20" s="0"/>
-      <c r="QP20" s="0"/>
-      <c r="QQ20" s="0"/>
-      <c r="QR20" s="0"/>
-      <c r="QS20" s="0"/>
-      <c r="QT20" s="0"/>
-      <c r="QU20" s="0"/>
-      <c r="QV20" s="0"/>
-      <c r="QW20" s="0"/>
-      <c r="QX20" s="0"/>
-      <c r="QY20" s="0"/>
-      <c r="QZ20" s="0"/>
-      <c r="RA20" s="0"/>
-      <c r="RB20" s="0"/>
-      <c r="RC20" s="0"/>
-      <c r="RD20" s="0"/>
-      <c r="RE20" s="0"/>
-      <c r="RF20" s="0"/>
-      <c r="RG20" s="0"/>
-      <c r="RH20" s="0"/>
-      <c r="RI20" s="0"/>
-      <c r="RJ20" s="0"/>
-      <c r="RK20" s="0"/>
-      <c r="RL20" s="0"/>
-      <c r="RM20" s="0"/>
-      <c r="RN20" s="0"/>
-      <c r="RO20" s="0"/>
-      <c r="RP20" s="0"/>
-      <c r="RQ20" s="0"/>
-      <c r="RR20" s="0"/>
-      <c r="RS20" s="0"/>
-      <c r="RT20" s="0"/>
-      <c r="RU20" s="0"/>
-      <c r="RV20" s="0"/>
-      <c r="RW20" s="0"/>
-      <c r="RX20" s="0"/>
-      <c r="RY20" s="0"/>
-      <c r="RZ20" s="0"/>
-      <c r="SA20" s="0"/>
-      <c r="SB20" s="0"/>
-      <c r="SC20" s="0"/>
-      <c r="SD20" s="0"/>
-      <c r="SE20" s="0"/>
-      <c r="SF20" s="0"/>
-      <c r="SG20" s="0"/>
-      <c r="SH20" s="0"/>
-      <c r="SI20" s="0"/>
-      <c r="SJ20" s="0"/>
-      <c r="SK20" s="0"/>
-      <c r="SL20" s="0"/>
-      <c r="SM20" s="0"/>
-      <c r="SN20" s="0"/>
-      <c r="SO20" s="0"/>
-      <c r="SP20" s="0"/>
-      <c r="SQ20" s="0"/>
-      <c r="SR20" s="0"/>
-      <c r="SS20" s="0"/>
-      <c r="ST20" s="0"/>
-      <c r="SU20" s="0"/>
-      <c r="SV20" s="0"/>
-      <c r="SW20" s="0"/>
-      <c r="SX20" s="0"/>
-      <c r="SY20" s="0"/>
-      <c r="SZ20" s="0"/>
-      <c r="TA20" s="0"/>
-      <c r="TB20" s="0"/>
-      <c r="TC20" s="0"/>
-      <c r="TD20" s="0"/>
-      <c r="TE20" s="0"/>
-      <c r="TF20" s="0"/>
-      <c r="TG20" s="0"/>
-      <c r="TH20" s="0"/>
-      <c r="TI20" s="0"/>
-      <c r="TJ20" s="0"/>
-      <c r="TK20" s="0"/>
-      <c r="TL20" s="0"/>
-      <c r="TM20" s="0"/>
-      <c r="TN20" s="0"/>
-      <c r="TO20" s="0"/>
-      <c r="TP20" s="0"/>
-      <c r="TQ20" s="0"/>
-      <c r="TR20" s="0"/>
-      <c r="TS20" s="0"/>
-      <c r="TT20" s="0"/>
-      <c r="TU20" s="0"/>
-      <c r="TV20" s="0"/>
-      <c r="TW20" s="0"/>
-      <c r="TX20" s="0"/>
-      <c r="TY20" s="0"/>
-      <c r="TZ20" s="0"/>
-      <c r="UA20" s="0"/>
-      <c r="UB20" s="0"/>
-      <c r="UC20" s="0"/>
-      <c r="UD20" s="0"/>
-      <c r="UE20" s="0"/>
-      <c r="UF20" s="0"/>
-      <c r="UG20" s="0"/>
-      <c r="UH20" s="0"/>
-      <c r="UI20" s="0"/>
-      <c r="UJ20" s="0"/>
-      <c r="UK20" s="0"/>
-      <c r="UL20" s="0"/>
-      <c r="UM20" s="0"/>
-      <c r="UN20" s="0"/>
-      <c r="UO20" s="0"/>
-      <c r="UP20" s="0"/>
-      <c r="UQ20" s="0"/>
-      <c r="UR20" s="0"/>
-      <c r="US20" s="0"/>
-      <c r="UT20" s="0"/>
-      <c r="UU20" s="0"/>
-      <c r="UV20" s="0"/>
-      <c r="UW20" s="0"/>
-      <c r="UX20" s="0"/>
-      <c r="UY20" s="0"/>
-      <c r="UZ20" s="0"/>
-      <c r="VA20" s="0"/>
-      <c r="VB20" s="0"/>
-      <c r="VC20" s="0"/>
-      <c r="VD20" s="0"/>
-      <c r="VE20" s="0"/>
-      <c r="VF20" s="0"/>
-      <c r="VG20" s="0"/>
-      <c r="VH20" s="0"/>
-      <c r="VI20" s="0"/>
-      <c r="VJ20" s="0"/>
-      <c r="VK20" s="0"/>
-      <c r="VL20" s="0"/>
-      <c r="VM20" s="0"/>
-      <c r="VN20" s="0"/>
-      <c r="VO20" s="0"/>
-      <c r="VP20" s="0"/>
-      <c r="VQ20" s="0"/>
-      <c r="VR20" s="0"/>
-      <c r="VS20" s="0"/>
-      <c r="VT20" s="0"/>
-      <c r="VU20" s="0"/>
-      <c r="VV20" s="0"/>
-      <c r="VW20" s="0"/>
-      <c r="VX20" s="0"/>
-      <c r="VY20" s="0"/>
-      <c r="VZ20" s="0"/>
-      <c r="WA20" s="0"/>
-      <c r="WB20" s="0"/>
-      <c r="WC20" s="0"/>
-      <c r="WD20" s="0"/>
-      <c r="WE20" s="0"/>
-      <c r="WF20" s="0"/>
-      <c r="WG20" s="0"/>
-      <c r="WH20" s="0"/>
-      <c r="WI20" s="0"/>
-      <c r="WJ20" s="0"/>
-      <c r="WK20" s="0"/>
-      <c r="WL20" s="0"/>
-      <c r="WM20" s="0"/>
-      <c r="WN20" s="0"/>
-      <c r="WO20" s="0"/>
-      <c r="WP20" s="0"/>
-      <c r="WQ20" s="0"/>
-      <c r="WR20" s="0"/>
-      <c r="WS20" s="0"/>
-      <c r="WT20" s="0"/>
-      <c r="WU20" s="0"/>
-      <c r="WV20" s="0"/>
-      <c r="WW20" s="0"/>
-      <c r="WX20" s="0"/>
-      <c r="WY20" s="0"/>
-      <c r="WZ20" s="0"/>
-      <c r="XA20" s="0"/>
-      <c r="XB20" s="0"/>
-      <c r="XC20" s="0"/>
-      <c r="XD20" s="0"/>
-      <c r="XE20" s="0"/>
-      <c r="XF20" s="0"/>
-      <c r="XG20" s="0"/>
-      <c r="XH20" s="0"/>
-      <c r="XI20" s="0"/>
-      <c r="XJ20" s="0"/>
-      <c r="XK20" s="0"/>
-      <c r="XL20" s="0"/>
-      <c r="XM20" s="0"/>
-      <c r="XN20" s="0"/>
-      <c r="XO20" s="0"/>
-      <c r="XP20" s="0"/>
-      <c r="XQ20" s="0"/>
-      <c r="XR20" s="0"/>
-      <c r="XS20" s="0"/>
-      <c r="XT20" s="0"/>
-      <c r="XU20" s="0"/>
-      <c r="XV20" s="0"/>
-      <c r="XW20" s="0"/>
-      <c r="XX20" s="0"/>
-      <c r="XY20" s="0"/>
-      <c r="XZ20" s="0"/>
-      <c r="YA20" s="0"/>
-      <c r="YB20" s="0"/>
-      <c r="YC20" s="0"/>
-      <c r="YD20" s="0"/>
-      <c r="YE20" s="0"/>
-      <c r="YF20" s="0"/>
-      <c r="YG20" s="0"/>
-      <c r="YH20" s="0"/>
-      <c r="YI20" s="0"/>
-      <c r="YJ20" s="0"/>
-      <c r="YK20" s="0"/>
-      <c r="YL20" s="0"/>
-      <c r="YM20" s="0"/>
-      <c r="YN20" s="0"/>
-      <c r="YO20" s="0"/>
-      <c r="YP20" s="0"/>
-      <c r="YQ20" s="0"/>
-      <c r="YR20" s="0"/>
-      <c r="YS20" s="0"/>
-      <c r="YT20" s="0"/>
-      <c r="YU20" s="0"/>
-      <c r="YV20" s="0"/>
-      <c r="YW20" s="0"/>
-      <c r="YX20" s="0"/>
-      <c r="YY20" s="0"/>
-      <c r="YZ20" s="0"/>
-      <c r="ZA20" s="0"/>
-      <c r="ZB20" s="0"/>
-      <c r="ZC20" s="0"/>
-      <c r="ZD20" s="0"/>
-      <c r="ZE20" s="0"/>
-      <c r="ZF20" s="0"/>
-      <c r="ZG20" s="0"/>
-      <c r="ZH20" s="0"/>
-      <c r="ZI20" s="0"/>
-      <c r="ZJ20" s="0"/>
-      <c r="ZK20" s="0"/>
-      <c r="ZL20" s="0"/>
-      <c r="ZM20" s="0"/>
-      <c r="ZN20" s="0"/>
-      <c r="ZO20" s="0"/>
-      <c r="ZP20" s="0"/>
-      <c r="ZQ20" s="0"/>
-      <c r="ZR20" s="0"/>
-      <c r="ZS20" s="0"/>
-      <c r="ZT20" s="0"/>
-      <c r="ZU20" s="0"/>
-      <c r="ZV20" s="0"/>
-      <c r="ZW20" s="0"/>
-      <c r="ZX20" s="0"/>
-      <c r="ZY20" s="0"/>
-      <c r="ZZ20" s="0"/>
-      <c r="AAA20" s="0"/>
-      <c r="AAB20" s="0"/>
-      <c r="AAC20" s="0"/>
-      <c r="AAD20" s="0"/>
-      <c r="AAE20" s="0"/>
-      <c r="AAF20" s="0"/>
-      <c r="AAG20" s="0"/>
-      <c r="AAH20" s="0"/>
-      <c r="AAI20" s="0"/>
-      <c r="AAJ20" s="0"/>
-      <c r="AAK20" s="0"/>
-      <c r="AAL20" s="0"/>
-      <c r="AAM20" s="0"/>
-      <c r="AAN20" s="0"/>
-      <c r="AAO20" s="0"/>
-      <c r="AAP20" s="0"/>
-      <c r="AAQ20" s="0"/>
-      <c r="AAR20" s="0"/>
-      <c r="AAS20" s="0"/>
-      <c r="AAT20" s="0"/>
-      <c r="AAU20" s="0"/>
-      <c r="AAV20" s="0"/>
-      <c r="AAW20" s="0"/>
-      <c r="AAX20" s="0"/>
-      <c r="AAY20" s="0"/>
-      <c r="AAZ20" s="0"/>
-      <c r="ABA20" s="0"/>
-      <c r="ABB20" s="0"/>
-      <c r="ABC20" s="0"/>
-      <c r="ABD20" s="0"/>
-      <c r="ABE20" s="0"/>
-      <c r="ABF20" s="0"/>
-      <c r="ABG20" s="0"/>
-      <c r="ABH20" s="0"/>
-      <c r="ABI20" s="0"/>
-      <c r="ABJ20" s="0"/>
-      <c r="ABK20" s="0"/>
-      <c r="ABL20" s="0"/>
-      <c r="ABM20" s="0"/>
-      <c r="ABN20" s="0"/>
-      <c r="ABO20" s="0"/>
-      <c r="ABP20" s="0"/>
-      <c r="ABQ20" s="0"/>
-      <c r="ABR20" s="0"/>
-      <c r="ABS20" s="0"/>
-      <c r="ABT20" s="0"/>
-      <c r="ABU20" s="0"/>
-      <c r="ABV20" s="0"/>
-      <c r="ABW20" s="0"/>
-      <c r="ABX20" s="0"/>
-      <c r="ABY20" s="0"/>
-      <c r="ABZ20" s="0"/>
-      <c r="ACA20" s="0"/>
-      <c r="ACB20" s="0"/>
-      <c r="ACC20" s="0"/>
-      <c r="ACD20" s="0"/>
-      <c r="ACE20" s="0"/>
-      <c r="ACF20" s="0"/>
-      <c r="ACG20" s="0"/>
-      <c r="ACH20" s="0"/>
-      <c r="ACI20" s="0"/>
-      <c r="ACJ20" s="0"/>
-      <c r="ACK20" s="0"/>
-      <c r="ACL20" s="0"/>
-      <c r="ACM20" s="0"/>
-      <c r="ACN20" s="0"/>
-      <c r="ACO20" s="0"/>
-      <c r="ACP20" s="0"/>
-      <c r="ACQ20" s="0"/>
-      <c r="ACR20" s="0"/>
-      <c r="ACS20" s="0"/>
-      <c r="ACT20" s="0"/>
-      <c r="ACU20" s="0"/>
-      <c r="ACV20" s="0"/>
-      <c r="ACW20" s="0"/>
-      <c r="ACX20" s="0"/>
-      <c r="ACY20" s="0"/>
-      <c r="ACZ20" s="0"/>
-      <c r="ADA20" s="0"/>
-      <c r="ADB20" s="0"/>
-      <c r="ADC20" s="0"/>
-      <c r="ADD20" s="0"/>
-      <c r="ADE20" s="0"/>
-      <c r="ADF20" s="0"/>
-      <c r="ADG20" s="0"/>
-      <c r="ADH20" s="0"/>
-      <c r="ADI20" s="0"/>
-      <c r="ADJ20" s="0"/>
-      <c r="ADK20" s="0"/>
-      <c r="ADL20" s="0"/>
-      <c r="ADM20" s="0"/>
-      <c r="ADN20" s="0"/>
-      <c r="ADO20" s="0"/>
-      <c r="ADP20" s="0"/>
-      <c r="ADQ20" s="0"/>
-      <c r="ADR20" s="0"/>
-      <c r="ADS20" s="0"/>
-      <c r="ADT20" s="0"/>
-      <c r="ADU20" s="0"/>
-      <c r="ADV20" s="0"/>
-      <c r="ADW20" s="0"/>
-      <c r="ADX20" s="0"/>
-      <c r="ADY20" s="0"/>
-      <c r="ADZ20" s="0"/>
-      <c r="AEA20" s="0"/>
-      <c r="AEB20" s="0"/>
-      <c r="AEC20" s="0"/>
-      <c r="AED20" s="0"/>
-      <c r="AEE20" s="0"/>
-      <c r="AEF20" s="0"/>
-      <c r="AEG20" s="0"/>
-      <c r="AEH20" s="0"/>
-      <c r="AEI20" s="0"/>
-      <c r="AEJ20" s="0"/>
-      <c r="AEK20" s="0"/>
-      <c r="AEL20" s="0"/>
-      <c r="AEM20" s="0"/>
-      <c r="AEN20" s="0"/>
-      <c r="AEO20" s="0"/>
-      <c r="AEP20" s="0"/>
-      <c r="AEQ20" s="0"/>
-      <c r="AER20" s="0"/>
-      <c r="AES20" s="0"/>
-      <c r="AET20" s="0"/>
-      <c r="AEU20" s="0"/>
-      <c r="AEV20" s="0"/>
-      <c r="AEW20" s="0"/>
-      <c r="AEX20" s="0"/>
-      <c r="AEY20" s="0"/>
-      <c r="AEZ20" s="0"/>
-      <c r="AFA20" s="0"/>
-      <c r="AFB20" s="0"/>
-      <c r="AFC20" s="0"/>
-      <c r="AFD20" s="0"/>
-      <c r="AFE20" s="0"/>
-      <c r="AFF20" s="0"/>
-      <c r="AFG20" s="0"/>
-      <c r="AFH20" s="0"/>
-      <c r="AFI20" s="0"/>
-      <c r="AFJ20" s="0"/>
-      <c r="AFK20" s="0"/>
-      <c r="AFL20" s="0"/>
-      <c r="AFM20" s="0"/>
-      <c r="AFN20" s="0"/>
-      <c r="AFO20" s="0"/>
-      <c r="AFP20" s="0"/>
-      <c r="AFQ20" s="0"/>
-      <c r="AFR20" s="0"/>
-      <c r="AFS20" s="0"/>
-      <c r="AFT20" s="0"/>
-      <c r="AFU20" s="0"/>
-      <c r="AFV20" s="0"/>
-      <c r="AFW20" s="0"/>
-      <c r="AFX20" s="0"/>
-      <c r="AFY20" s="0"/>
-      <c r="AFZ20" s="0"/>
-      <c r="AGA20" s="0"/>
-      <c r="AGB20" s="0"/>
-      <c r="AGC20" s="0"/>
-      <c r="AGD20" s="0"/>
-      <c r="AGE20" s="0"/>
-      <c r="AGF20" s="0"/>
-      <c r="AGG20" s="0"/>
-      <c r="AGH20" s="0"/>
-      <c r="AGI20" s="0"/>
-      <c r="AGJ20" s="0"/>
-      <c r="AGK20" s="0"/>
-      <c r="AGL20" s="0"/>
-      <c r="AGM20" s="0"/>
-      <c r="AGN20" s="0"/>
-      <c r="AGO20" s="0"/>
-      <c r="AGP20" s="0"/>
-      <c r="AGQ20" s="0"/>
-      <c r="AGR20" s="0"/>
-      <c r="AGS20" s="0"/>
-      <c r="AGT20" s="0"/>
-      <c r="AGU20" s="0"/>
-      <c r="AGV20" s="0"/>
-      <c r="AGW20" s="0"/>
-      <c r="AGX20" s="0"/>
-      <c r="AGY20" s="0"/>
-      <c r="AGZ20" s="0"/>
-      <c r="AHA20" s="0"/>
-      <c r="AHB20" s="0"/>
-      <c r="AHC20" s="0"/>
-      <c r="AHD20" s="0"/>
-      <c r="AHE20" s="0"/>
-      <c r="AHF20" s="0"/>
-      <c r="AHG20" s="0"/>
-      <c r="AHH20" s="0"/>
-      <c r="AHI20" s="0"/>
-      <c r="AHJ20" s="0"/>
-      <c r="AHK20" s="0"/>
-      <c r="AHL20" s="0"/>
-      <c r="AHM20" s="0"/>
-      <c r="AHN20" s="0"/>
-      <c r="AHO20" s="0"/>
-      <c r="AHP20" s="0"/>
-      <c r="AHQ20" s="0"/>
-      <c r="AHR20" s="0"/>
-      <c r="AHS20" s="0"/>
-      <c r="AHT20" s="0"/>
-      <c r="AHU20" s="0"/>
-      <c r="AHV20" s="0"/>
-      <c r="AHW20" s="0"/>
-      <c r="AHX20" s="0"/>
-      <c r="AHY20" s="0"/>
-      <c r="AHZ20" s="0"/>
-      <c r="AIA20" s="0"/>
-      <c r="AIB20" s="0"/>
-      <c r="AIC20" s="0"/>
-      <c r="AID20" s="0"/>
-      <c r="AIE20" s="0"/>
-      <c r="AIF20" s="0"/>
-      <c r="AIG20" s="0"/>
-      <c r="AIH20" s="0"/>
-      <c r="AII20" s="0"/>
-      <c r="AIJ20" s="0"/>
-      <c r="AIK20" s="0"/>
-      <c r="AIL20" s="0"/>
-      <c r="AIM20" s="0"/>
-      <c r="AIN20" s="0"/>
-      <c r="AIO20" s="0"/>
-      <c r="AIP20" s="0"/>
-      <c r="AIQ20" s="0"/>
-      <c r="AIR20" s="0"/>
-      <c r="AIS20" s="0"/>
-      <c r="AIT20" s="0"/>
-      <c r="AIU20" s="0"/>
-      <c r="AIV20" s="0"/>
-      <c r="AIW20" s="0"/>
-      <c r="AIX20" s="0"/>
-      <c r="AIY20" s="0"/>
-      <c r="AIZ20" s="0"/>
-      <c r="AJA20" s="0"/>
-      <c r="AJB20" s="0"/>
-      <c r="AJC20" s="0"/>
-      <c r="AJD20" s="0"/>
-      <c r="AJE20" s="0"/>
-      <c r="AJF20" s="0"/>
-      <c r="AJG20" s="0"/>
-      <c r="AJH20" s="0"/>
-      <c r="AJI20" s="0"/>
-      <c r="AJJ20" s="0"/>
-      <c r="AJK20" s="0"/>
-      <c r="AJL20" s="0"/>
-      <c r="AJM20" s="0"/>
-      <c r="AJN20" s="0"/>
-      <c r="AJO20" s="0"/>
-      <c r="AJP20" s="0"/>
-      <c r="AJQ20" s="0"/>
-      <c r="AJR20" s="0"/>
-      <c r="AJS20" s="0"/>
-      <c r="AJT20" s="0"/>
-      <c r="AJU20" s="0"/>
-      <c r="AJV20" s="0"/>
-      <c r="AJW20" s="0"/>
-      <c r="AJX20" s="0"/>
-      <c r="AJY20" s="0"/>
-      <c r="AJZ20" s="0"/>
-      <c r="AKA20" s="0"/>
-      <c r="AKB20" s="0"/>
-      <c r="AKC20" s="0"/>
-      <c r="AKD20" s="0"/>
-      <c r="AKE20" s="0"/>
-      <c r="AKF20" s="0"/>
-      <c r="AKG20" s="0"/>
-      <c r="AKH20" s="0"/>
-      <c r="AKI20" s="0"/>
-      <c r="AKJ20" s="0"/>
-      <c r="AKK20" s="0"/>
-      <c r="AKL20" s="0"/>
-      <c r="AKM20" s="0"/>
-      <c r="AKN20" s="0"/>
-      <c r="AKO20" s="0"/>
-      <c r="AKP20" s="0"/>
-      <c r="AKQ20" s="0"/>
-      <c r="AKR20" s="0"/>
-      <c r="AKS20" s="0"/>
-      <c r="AKT20" s="0"/>
-      <c r="AKU20" s="0"/>
-      <c r="AKV20" s="0"/>
-      <c r="AKW20" s="0"/>
-      <c r="AKX20" s="0"/>
-      <c r="AKY20" s="0"/>
-      <c r="AKZ20" s="0"/>
-      <c r="ALA20" s="0"/>
-      <c r="ALB20" s="0"/>
-      <c r="ALC20" s="0"/>
-      <c r="ALD20" s="0"/>
-      <c r="ALE20" s="0"/>
-      <c r="ALF20" s="0"/>
-      <c r="ALG20" s="0"/>
-      <c r="ALH20" s="0"/>
-      <c r="ALI20" s="0"/>
-      <c r="ALJ20" s="0"/>
-      <c r="ALK20" s="0"/>
-      <c r="ALL20" s="0"/>
-      <c r="ALM20" s="0"/>
-      <c r="ALN20" s="0"/>
-      <c r="ALO20" s="0"/>
-      <c r="ALP20" s="0"/>
-      <c r="ALQ20" s="0"/>
-      <c r="ALR20" s="0"/>
-      <c r="ALS20" s="0"/>
-      <c r="ALT20" s="0"/>
-      <c r="ALU20" s="0"/>
-      <c r="ALV20" s="0"/>
-      <c r="ALW20" s="0"/>
-      <c r="ALX20" s="0"/>
-      <c r="ALY20" s="0"/>
-      <c r="ALZ20" s="0"/>
-      <c r="AMA20" s="0"/>
-      <c r="AMB20" s="0"/>
-      <c r="AMC20" s="0"/>
-      <c r="AMD20" s="0"/>
-      <c r="AME20" s="0"/>
-      <c r="AMF20" s="0"/>
-      <c r="AMG20" s="0"/>
-      <c r="AMH20" s="0"/>
-      <c r="AMI20" s="0"/>
-      <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="E21" s="7" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="9" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="J21" s="10"/>
       <c r="L21" s="0"/>
@@ -3174,27 +2236,29 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="7"/>
+      <c r="D22" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="E22" s="7" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="9" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J22" s="10"/>
       <c r="L22" s="0"/>
@@ -4213,134 +3277,1171 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="E23" s="7" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="9" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="J23" s="10"/>
+      <c r="L23" s="0"/>
+      <c r="M23" s="0"/>
+      <c r="N23" s="0"/>
+      <c r="O23" s="0"/>
+      <c r="P23" s="0"/>
+      <c r="Q23" s="0"/>
+      <c r="R23" s="0"/>
+      <c r="S23" s="0"/>
+      <c r="T23" s="0"/>
+      <c r="U23" s="0"/>
+      <c r="V23" s="0"/>
+      <c r="W23" s="0"/>
+      <c r="X23" s="0"/>
+      <c r="Y23" s="0"/>
+      <c r="Z23" s="0"/>
+      <c r="AA23" s="0"/>
+      <c r="AB23" s="0"/>
+      <c r="AC23" s="0"/>
+      <c r="AD23" s="0"/>
+      <c r="AE23" s="0"/>
+      <c r="AF23" s="0"/>
+      <c r="AG23" s="0"/>
+      <c r="AH23" s="0"/>
+      <c r="AI23" s="0"/>
+      <c r="AJ23" s="0"/>
+      <c r="AK23" s="0"/>
+      <c r="AL23" s="0"/>
+      <c r="AM23" s="0"/>
+      <c r="AN23" s="0"/>
+      <c r="AO23" s="0"/>
+      <c r="AP23" s="0"/>
+      <c r="AQ23" s="0"/>
+      <c r="AR23" s="0"/>
+      <c r="AS23" s="0"/>
+      <c r="AT23" s="0"/>
+      <c r="AU23" s="0"/>
+      <c r="AV23" s="0"/>
+      <c r="AW23" s="0"/>
+      <c r="AX23" s="0"/>
+      <c r="AY23" s="0"/>
+      <c r="AZ23" s="0"/>
+      <c r="BA23" s="0"/>
+      <c r="BB23" s="0"/>
+      <c r="BC23" s="0"/>
+      <c r="BD23" s="0"/>
+      <c r="BE23" s="0"/>
+      <c r="BF23" s="0"/>
+      <c r="BG23" s="0"/>
+      <c r="BH23" s="0"/>
+      <c r="BI23" s="0"/>
+      <c r="BJ23" s="0"/>
+      <c r="BK23" s="0"/>
+      <c r="BL23" s="0"/>
+      <c r="BM23" s="0"/>
+      <c r="BN23" s="0"/>
+      <c r="BO23" s="0"/>
+      <c r="BP23" s="0"/>
+      <c r="BQ23" s="0"/>
+      <c r="BR23" s="0"/>
+      <c r="BS23" s="0"/>
+      <c r="BT23" s="0"/>
+      <c r="BU23" s="0"/>
+      <c r="BV23" s="0"/>
+      <c r="BW23" s="0"/>
+      <c r="BX23" s="0"/>
+      <c r="BY23" s="0"/>
+      <c r="BZ23" s="0"/>
+      <c r="CA23" s="0"/>
+      <c r="CB23" s="0"/>
+      <c r="CC23" s="0"/>
+      <c r="CD23" s="0"/>
+      <c r="CE23" s="0"/>
+      <c r="CF23" s="0"/>
+      <c r="CG23" s="0"/>
+      <c r="CH23" s="0"/>
+      <c r="CI23" s="0"/>
+      <c r="CJ23" s="0"/>
+      <c r="CK23" s="0"/>
+      <c r="CL23" s="0"/>
+      <c r="CM23" s="0"/>
+      <c r="CN23" s="0"/>
+      <c r="CO23" s="0"/>
+      <c r="CP23" s="0"/>
+      <c r="CQ23" s="0"/>
+      <c r="CR23" s="0"/>
+      <c r="CS23" s="0"/>
+      <c r="CT23" s="0"/>
+      <c r="CU23" s="0"/>
+      <c r="CV23" s="0"/>
+      <c r="CW23" s="0"/>
+      <c r="CX23" s="0"/>
+      <c r="CY23" s="0"/>
+      <c r="CZ23" s="0"/>
+      <c r="DA23" s="0"/>
+      <c r="DB23" s="0"/>
+      <c r="DC23" s="0"/>
+      <c r="DD23" s="0"/>
+      <c r="DE23" s="0"/>
+      <c r="DF23" s="0"/>
+      <c r="DG23" s="0"/>
+      <c r="DH23" s="0"/>
+      <c r="DI23" s="0"/>
+      <c r="DJ23" s="0"/>
+      <c r="DK23" s="0"/>
+      <c r="DL23" s="0"/>
+      <c r="DM23" s="0"/>
+      <c r="DN23" s="0"/>
+      <c r="DO23" s="0"/>
+      <c r="DP23" s="0"/>
+      <c r="DQ23" s="0"/>
+      <c r="DR23" s="0"/>
+      <c r="DS23" s="0"/>
+      <c r="DT23" s="0"/>
+      <c r="DU23" s="0"/>
+      <c r="DV23" s="0"/>
+      <c r="DW23" s="0"/>
+      <c r="DX23" s="0"/>
+      <c r="DY23" s="0"/>
+      <c r="DZ23" s="0"/>
+      <c r="EA23" s="0"/>
+      <c r="EB23" s="0"/>
+      <c r="EC23" s="0"/>
+      <c r="ED23" s="0"/>
+      <c r="EE23" s="0"/>
+      <c r="EF23" s="0"/>
+      <c r="EG23" s="0"/>
+      <c r="EH23" s="0"/>
+      <c r="EI23" s="0"/>
+      <c r="EJ23" s="0"/>
+      <c r="EK23" s="0"/>
+      <c r="EL23" s="0"/>
+      <c r="EM23" s="0"/>
+      <c r="EN23" s="0"/>
+      <c r="EO23" s="0"/>
+      <c r="EP23" s="0"/>
+      <c r="EQ23" s="0"/>
+      <c r="ER23" s="0"/>
+      <c r="ES23" s="0"/>
+      <c r="ET23" s="0"/>
+      <c r="EU23" s="0"/>
+      <c r="EV23" s="0"/>
+      <c r="EW23" s="0"/>
+      <c r="EX23" s="0"/>
+      <c r="EY23" s="0"/>
+      <c r="EZ23" s="0"/>
+      <c r="FA23" s="0"/>
+      <c r="FB23" s="0"/>
+      <c r="FC23" s="0"/>
+      <c r="FD23" s="0"/>
+      <c r="FE23" s="0"/>
+      <c r="FF23" s="0"/>
+      <c r="FG23" s="0"/>
+      <c r="FH23" s="0"/>
+      <c r="FI23" s="0"/>
+      <c r="FJ23" s="0"/>
+      <c r="FK23" s="0"/>
+      <c r="FL23" s="0"/>
+      <c r="FM23" s="0"/>
+      <c r="FN23" s="0"/>
+      <c r="FO23" s="0"/>
+      <c r="FP23" s="0"/>
+      <c r="FQ23" s="0"/>
+      <c r="FR23" s="0"/>
+      <c r="FS23" s="0"/>
+      <c r="FT23" s="0"/>
+      <c r="FU23" s="0"/>
+      <c r="FV23" s="0"/>
+      <c r="FW23" s="0"/>
+      <c r="FX23" s="0"/>
+      <c r="FY23" s="0"/>
+      <c r="FZ23" s="0"/>
+      <c r="GA23" s="0"/>
+      <c r="GB23" s="0"/>
+      <c r="GC23" s="0"/>
+      <c r="GD23" s="0"/>
+      <c r="GE23" s="0"/>
+      <c r="GF23" s="0"/>
+      <c r="GG23" s="0"/>
+      <c r="GH23" s="0"/>
+      <c r="GI23" s="0"/>
+      <c r="GJ23" s="0"/>
+      <c r="GK23" s="0"/>
+      <c r="GL23" s="0"/>
+      <c r="GM23" s="0"/>
+      <c r="GN23" s="0"/>
+      <c r="GO23" s="0"/>
+      <c r="GP23" s="0"/>
+      <c r="GQ23" s="0"/>
+      <c r="GR23" s="0"/>
+      <c r="GS23" s="0"/>
+      <c r="GT23" s="0"/>
+      <c r="GU23" s="0"/>
+      <c r="GV23" s="0"/>
+      <c r="GW23" s="0"/>
+      <c r="GX23" s="0"/>
+      <c r="GY23" s="0"/>
+      <c r="GZ23" s="0"/>
+      <c r="HA23" s="0"/>
+      <c r="HB23" s="0"/>
+      <c r="HC23" s="0"/>
+      <c r="HD23" s="0"/>
+      <c r="HE23" s="0"/>
+      <c r="HF23" s="0"/>
+      <c r="HG23" s="0"/>
+      <c r="HH23" s="0"/>
+      <c r="HI23" s="0"/>
+      <c r="HJ23" s="0"/>
+      <c r="HK23" s="0"/>
+      <c r="HL23" s="0"/>
+      <c r="HM23" s="0"/>
+      <c r="HN23" s="0"/>
+      <c r="HO23" s="0"/>
+      <c r="HP23" s="0"/>
+      <c r="HQ23" s="0"/>
+      <c r="HR23" s="0"/>
+      <c r="HS23" s="0"/>
+      <c r="HT23" s="0"/>
+      <c r="HU23" s="0"/>
+      <c r="HV23" s="0"/>
+      <c r="HW23" s="0"/>
+      <c r="HX23" s="0"/>
+      <c r="HY23" s="0"/>
+      <c r="HZ23" s="0"/>
+      <c r="IA23" s="0"/>
+      <c r="IB23" s="0"/>
+      <c r="IC23" s="0"/>
+      <c r="ID23" s="0"/>
+      <c r="IE23" s="0"/>
+      <c r="IF23" s="0"/>
+      <c r="IG23" s="0"/>
+      <c r="IH23" s="0"/>
+      <c r="II23" s="0"/>
+      <c r="IJ23" s="0"/>
+      <c r="IK23" s="0"/>
+      <c r="IL23" s="0"/>
+      <c r="IM23" s="0"/>
+      <c r="IN23" s="0"/>
+      <c r="IO23" s="0"/>
+      <c r="IP23" s="0"/>
+      <c r="IQ23" s="0"/>
+      <c r="IR23" s="0"/>
+      <c r="IS23" s="0"/>
+      <c r="IT23" s="0"/>
+      <c r="IU23" s="0"/>
+      <c r="IV23" s="0"/>
+      <c r="IW23" s="0"/>
+      <c r="IX23" s="0"/>
+      <c r="IY23" s="0"/>
+      <c r="IZ23" s="0"/>
+      <c r="JA23" s="0"/>
+      <c r="JB23" s="0"/>
+      <c r="JC23" s="0"/>
+      <c r="JD23" s="0"/>
+      <c r="JE23" s="0"/>
+      <c r="JF23" s="0"/>
+      <c r="JG23" s="0"/>
+      <c r="JH23" s="0"/>
+      <c r="JI23" s="0"/>
+      <c r="JJ23" s="0"/>
+      <c r="JK23" s="0"/>
+      <c r="JL23" s="0"/>
+      <c r="JM23" s="0"/>
+      <c r="JN23" s="0"/>
+      <c r="JO23" s="0"/>
+      <c r="JP23" s="0"/>
+      <c r="JQ23" s="0"/>
+      <c r="JR23" s="0"/>
+      <c r="JS23" s="0"/>
+      <c r="JT23" s="0"/>
+      <c r="JU23" s="0"/>
+      <c r="JV23" s="0"/>
+      <c r="JW23" s="0"/>
+      <c r="JX23" s="0"/>
+      <c r="JY23" s="0"/>
+      <c r="JZ23" s="0"/>
+      <c r="KA23" s="0"/>
+      <c r="KB23" s="0"/>
+      <c r="KC23" s="0"/>
+      <c r="KD23" s="0"/>
+      <c r="KE23" s="0"/>
+      <c r="KF23" s="0"/>
+      <c r="KG23" s="0"/>
+      <c r="KH23" s="0"/>
+      <c r="KI23" s="0"/>
+      <c r="KJ23" s="0"/>
+      <c r="KK23" s="0"/>
+      <c r="KL23" s="0"/>
+      <c r="KM23" s="0"/>
+      <c r="KN23" s="0"/>
+      <c r="KO23" s="0"/>
+      <c r="KP23" s="0"/>
+      <c r="KQ23" s="0"/>
+      <c r="KR23" s="0"/>
+      <c r="KS23" s="0"/>
+      <c r="KT23" s="0"/>
+      <c r="KU23" s="0"/>
+      <c r="KV23" s="0"/>
+      <c r="KW23" s="0"/>
+      <c r="KX23" s="0"/>
+      <c r="KY23" s="0"/>
+      <c r="KZ23" s="0"/>
+      <c r="LA23" s="0"/>
+      <c r="LB23" s="0"/>
+      <c r="LC23" s="0"/>
+      <c r="LD23" s="0"/>
+      <c r="LE23" s="0"/>
+      <c r="LF23" s="0"/>
+      <c r="LG23" s="0"/>
+      <c r="LH23" s="0"/>
+      <c r="LI23" s="0"/>
+      <c r="LJ23" s="0"/>
+      <c r="LK23" s="0"/>
+      <c r="LL23" s="0"/>
+      <c r="LM23" s="0"/>
+      <c r="LN23" s="0"/>
+      <c r="LO23" s="0"/>
+      <c r="LP23" s="0"/>
+      <c r="LQ23" s="0"/>
+      <c r="LR23" s="0"/>
+      <c r="LS23" s="0"/>
+      <c r="LT23" s="0"/>
+      <c r="LU23" s="0"/>
+      <c r="LV23" s="0"/>
+      <c r="LW23" s="0"/>
+      <c r="LX23" s="0"/>
+      <c r="LY23" s="0"/>
+      <c r="LZ23" s="0"/>
+      <c r="MA23" s="0"/>
+      <c r="MB23" s="0"/>
+      <c r="MC23" s="0"/>
+      <c r="MD23" s="0"/>
+      <c r="ME23" s="0"/>
+      <c r="MF23" s="0"/>
+      <c r="MG23" s="0"/>
+      <c r="MH23" s="0"/>
+      <c r="MI23" s="0"/>
+      <c r="MJ23" s="0"/>
+      <c r="MK23" s="0"/>
+      <c r="ML23" s="0"/>
+      <c r="MM23" s="0"/>
+      <c r="MN23" s="0"/>
+      <c r="MO23" s="0"/>
+      <c r="MP23" s="0"/>
+      <c r="MQ23" s="0"/>
+      <c r="MR23" s="0"/>
+      <c r="MS23" s="0"/>
+      <c r="MT23" s="0"/>
+      <c r="MU23" s="0"/>
+      <c r="MV23" s="0"/>
+      <c r="MW23" s="0"/>
+      <c r="MX23" s="0"/>
+      <c r="MY23" s="0"/>
+      <c r="MZ23" s="0"/>
+      <c r="NA23" s="0"/>
+      <c r="NB23" s="0"/>
+      <c r="NC23" s="0"/>
+      <c r="ND23" s="0"/>
+      <c r="NE23" s="0"/>
+      <c r="NF23" s="0"/>
+      <c r="NG23" s="0"/>
+      <c r="NH23" s="0"/>
+      <c r="NI23" s="0"/>
+      <c r="NJ23" s="0"/>
+      <c r="NK23" s="0"/>
+      <c r="NL23" s="0"/>
+      <c r="NM23" s="0"/>
+      <c r="NN23" s="0"/>
+      <c r="NO23" s="0"/>
+      <c r="NP23" s="0"/>
+      <c r="NQ23" s="0"/>
+      <c r="NR23" s="0"/>
+      <c r="NS23" s="0"/>
+      <c r="NT23" s="0"/>
+      <c r="NU23" s="0"/>
+      <c r="NV23" s="0"/>
+      <c r="NW23" s="0"/>
+      <c r="NX23" s="0"/>
+      <c r="NY23" s="0"/>
+      <c r="NZ23" s="0"/>
+      <c r="OA23" s="0"/>
+      <c r="OB23" s="0"/>
+      <c r="OC23" s="0"/>
+      <c r="OD23" s="0"/>
+      <c r="OE23" s="0"/>
+      <c r="OF23" s="0"/>
+      <c r="OG23" s="0"/>
+      <c r="OH23" s="0"/>
+      <c r="OI23" s="0"/>
+      <c r="OJ23" s="0"/>
+      <c r="OK23" s="0"/>
+      <c r="OL23" s="0"/>
+      <c r="OM23" s="0"/>
+      <c r="ON23" s="0"/>
+      <c r="OO23" s="0"/>
+      <c r="OP23" s="0"/>
+      <c r="OQ23" s="0"/>
+      <c r="OR23" s="0"/>
+      <c r="OS23" s="0"/>
+      <c r="OT23" s="0"/>
+      <c r="OU23" s="0"/>
+      <c r="OV23" s="0"/>
+      <c r="OW23" s="0"/>
+      <c r="OX23" s="0"/>
+      <c r="OY23" s="0"/>
+      <c r="OZ23" s="0"/>
+      <c r="PA23" s="0"/>
+      <c r="PB23" s="0"/>
+      <c r="PC23" s="0"/>
+      <c r="PD23" s="0"/>
+      <c r="PE23" s="0"/>
+      <c r="PF23" s="0"/>
+      <c r="PG23" s="0"/>
+      <c r="PH23" s="0"/>
+      <c r="PI23" s="0"/>
+      <c r="PJ23" s="0"/>
+      <c r="PK23" s="0"/>
+      <c r="PL23" s="0"/>
+      <c r="PM23" s="0"/>
+      <c r="PN23" s="0"/>
+      <c r="PO23" s="0"/>
+      <c r="PP23" s="0"/>
+      <c r="PQ23" s="0"/>
+      <c r="PR23" s="0"/>
+      <c r="PS23" s="0"/>
+      <c r="PT23" s="0"/>
+      <c r="PU23" s="0"/>
+      <c r="PV23" s="0"/>
+      <c r="PW23" s="0"/>
+      <c r="PX23" s="0"/>
+      <c r="PY23" s="0"/>
+      <c r="PZ23" s="0"/>
+      <c r="QA23" s="0"/>
+      <c r="QB23" s="0"/>
+      <c r="QC23" s="0"/>
+      <c r="QD23" s="0"/>
+      <c r="QE23" s="0"/>
+      <c r="QF23" s="0"/>
+      <c r="QG23" s="0"/>
+      <c r="QH23" s="0"/>
+      <c r="QI23" s="0"/>
+      <c r="QJ23" s="0"/>
+      <c r="QK23" s="0"/>
+      <c r="QL23" s="0"/>
+      <c r="QM23" s="0"/>
+      <c r="QN23" s="0"/>
+      <c r="QO23" s="0"/>
+      <c r="QP23" s="0"/>
+      <c r="QQ23" s="0"/>
+      <c r="QR23" s="0"/>
+      <c r="QS23" s="0"/>
+      <c r="QT23" s="0"/>
+      <c r="QU23" s="0"/>
+      <c r="QV23" s="0"/>
+      <c r="QW23" s="0"/>
+      <c r="QX23" s="0"/>
+      <c r="QY23" s="0"/>
+      <c r="QZ23" s="0"/>
+      <c r="RA23" s="0"/>
+      <c r="RB23" s="0"/>
+      <c r="RC23" s="0"/>
+      <c r="RD23" s="0"/>
+      <c r="RE23" s="0"/>
+      <c r="RF23" s="0"/>
+      <c r="RG23" s="0"/>
+      <c r="RH23" s="0"/>
+      <c r="RI23" s="0"/>
+      <c r="RJ23" s="0"/>
+      <c r="RK23" s="0"/>
+      <c r="RL23" s="0"/>
+      <c r="RM23" s="0"/>
+      <c r="RN23" s="0"/>
+      <c r="RO23" s="0"/>
+      <c r="RP23" s="0"/>
+      <c r="RQ23" s="0"/>
+      <c r="RR23" s="0"/>
+      <c r="RS23" s="0"/>
+      <c r="RT23" s="0"/>
+      <c r="RU23" s="0"/>
+      <c r="RV23" s="0"/>
+      <c r="RW23" s="0"/>
+      <c r="RX23" s="0"/>
+      <c r="RY23" s="0"/>
+      <c r="RZ23" s="0"/>
+      <c r="SA23" s="0"/>
+      <c r="SB23" s="0"/>
+      <c r="SC23" s="0"/>
+      <c r="SD23" s="0"/>
+      <c r="SE23" s="0"/>
+      <c r="SF23" s="0"/>
+      <c r="SG23" s="0"/>
+      <c r="SH23" s="0"/>
+      <c r="SI23" s="0"/>
+      <c r="SJ23" s="0"/>
+      <c r="SK23" s="0"/>
+      <c r="SL23" s="0"/>
+      <c r="SM23" s="0"/>
+      <c r="SN23" s="0"/>
+      <c r="SO23" s="0"/>
+      <c r="SP23" s="0"/>
+      <c r="SQ23" s="0"/>
+      <c r="SR23" s="0"/>
+      <c r="SS23" s="0"/>
+      <c r="ST23" s="0"/>
+      <c r="SU23" s="0"/>
+      <c r="SV23" s="0"/>
+      <c r="SW23" s="0"/>
+      <c r="SX23" s="0"/>
+      <c r="SY23" s="0"/>
+      <c r="SZ23" s="0"/>
+      <c r="TA23" s="0"/>
+      <c r="TB23" s="0"/>
+      <c r="TC23" s="0"/>
+      <c r="TD23" s="0"/>
+      <c r="TE23" s="0"/>
+      <c r="TF23" s="0"/>
+      <c r="TG23" s="0"/>
+      <c r="TH23" s="0"/>
+      <c r="TI23" s="0"/>
+      <c r="TJ23" s="0"/>
+      <c r="TK23" s="0"/>
+      <c r="TL23" s="0"/>
+      <c r="TM23" s="0"/>
+      <c r="TN23" s="0"/>
+      <c r="TO23" s="0"/>
+      <c r="TP23" s="0"/>
+      <c r="TQ23" s="0"/>
+      <c r="TR23" s="0"/>
+      <c r="TS23" s="0"/>
+      <c r="TT23" s="0"/>
+      <c r="TU23" s="0"/>
+      <c r="TV23" s="0"/>
+      <c r="TW23" s="0"/>
+      <c r="TX23" s="0"/>
+      <c r="TY23" s="0"/>
+      <c r="TZ23" s="0"/>
+      <c r="UA23" s="0"/>
+      <c r="UB23" s="0"/>
+      <c r="UC23" s="0"/>
+      <c r="UD23" s="0"/>
+      <c r="UE23" s="0"/>
+      <c r="UF23" s="0"/>
+      <c r="UG23" s="0"/>
+      <c r="UH23" s="0"/>
+      <c r="UI23" s="0"/>
+      <c r="UJ23" s="0"/>
+      <c r="UK23" s="0"/>
+      <c r="UL23" s="0"/>
+      <c r="UM23" s="0"/>
+      <c r="UN23" s="0"/>
+      <c r="UO23" s="0"/>
+      <c r="UP23" s="0"/>
+      <c r="UQ23" s="0"/>
+      <c r="UR23" s="0"/>
+      <c r="US23" s="0"/>
+      <c r="UT23" s="0"/>
+      <c r="UU23" s="0"/>
+      <c r="UV23" s="0"/>
+      <c r="UW23" s="0"/>
+      <c r="UX23" s="0"/>
+      <c r="UY23" s="0"/>
+      <c r="UZ23" s="0"/>
+      <c r="VA23" s="0"/>
+      <c r="VB23" s="0"/>
+      <c r="VC23" s="0"/>
+      <c r="VD23" s="0"/>
+      <c r="VE23" s="0"/>
+      <c r="VF23" s="0"/>
+      <c r="VG23" s="0"/>
+      <c r="VH23" s="0"/>
+      <c r="VI23" s="0"/>
+      <c r="VJ23" s="0"/>
+      <c r="VK23" s="0"/>
+      <c r="VL23" s="0"/>
+      <c r="VM23" s="0"/>
+      <c r="VN23" s="0"/>
+      <c r="VO23" s="0"/>
+      <c r="VP23" s="0"/>
+      <c r="VQ23" s="0"/>
+      <c r="VR23" s="0"/>
+      <c r="VS23" s="0"/>
+      <c r="VT23" s="0"/>
+      <c r="VU23" s="0"/>
+      <c r="VV23" s="0"/>
+      <c r="VW23" s="0"/>
+      <c r="VX23" s="0"/>
+      <c r="VY23" s="0"/>
+      <c r="VZ23" s="0"/>
+      <c r="WA23" s="0"/>
+      <c r="WB23" s="0"/>
+      <c r="WC23" s="0"/>
+      <c r="WD23" s="0"/>
+      <c r="WE23" s="0"/>
+      <c r="WF23" s="0"/>
+      <c r="WG23" s="0"/>
+      <c r="WH23" s="0"/>
+      <c r="WI23" s="0"/>
+      <c r="WJ23" s="0"/>
+      <c r="WK23" s="0"/>
+      <c r="WL23" s="0"/>
+      <c r="WM23" s="0"/>
+      <c r="WN23" s="0"/>
+      <c r="WO23" s="0"/>
+      <c r="WP23" s="0"/>
+      <c r="WQ23" s="0"/>
+      <c r="WR23" s="0"/>
+      <c r="WS23" s="0"/>
+      <c r="WT23" s="0"/>
+      <c r="WU23" s="0"/>
+      <c r="WV23" s="0"/>
+      <c r="WW23" s="0"/>
+      <c r="WX23" s="0"/>
+      <c r="WY23" s="0"/>
+      <c r="WZ23" s="0"/>
+      <c r="XA23" s="0"/>
+      <c r="XB23" s="0"/>
+      <c r="XC23" s="0"/>
+      <c r="XD23" s="0"/>
+      <c r="XE23" s="0"/>
+      <c r="XF23" s="0"/>
+      <c r="XG23" s="0"/>
+      <c r="XH23" s="0"/>
+      <c r="XI23" s="0"/>
+      <c r="XJ23" s="0"/>
+      <c r="XK23" s="0"/>
+      <c r="XL23" s="0"/>
+      <c r="XM23" s="0"/>
+      <c r="XN23" s="0"/>
+      <c r="XO23" s="0"/>
+      <c r="XP23" s="0"/>
+      <c r="XQ23" s="0"/>
+      <c r="XR23" s="0"/>
+      <c r="XS23" s="0"/>
+      <c r="XT23" s="0"/>
+      <c r="XU23" s="0"/>
+      <c r="XV23" s="0"/>
+      <c r="XW23" s="0"/>
+      <c r="XX23" s="0"/>
+      <c r="XY23" s="0"/>
+      <c r="XZ23" s="0"/>
+      <c r="YA23" s="0"/>
+      <c r="YB23" s="0"/>
+      <c r="YC23" s="0"/>
+      <c r="YD23" s="0"/>
+      <c r="YE23" s="0"/>
+      <c r="YF23" s="0"/>
+      <c r="YG23" s="0"/>
+      <c r="YH23" s="0"/>
+      <c r="YI23" s="0"/>
+      <c r="YJ23" s="0"/>
+      <c r="YK23" s="0"/>
+      <c r="YL23" s="0"/>
+      <c r="YM23" s="0"/>
+      <c r="YN23" s="0"/>
+      <c r="YO23" s="0"/>
+      <c r="YP23" s="0"/>
+      <c r="YQ23" s="0"/>
+      <c r="YR23" s="0"/>
+      <c r="YS23" s="0"/>
+      <c r="YT23" s="0"/>
+      <c r="YU23" s="0"/>
+      <c r="YV23" s="0"/>
+      <c r="YW23" s="0"/>
+      <c r="YX23" s="0"/>
+      <c r="YY23" s="0"/>
+      <c r="YZ23" s="0"/>
+      <c r="ZA23" s="0"/>
+      <c r="ZB23" s="0"/>
+      <c r="ZC23" s="0"/>
+      <c r="ZD23" s="0"/>
+      <c r="ZE23" s="0"/>
+      <c r="ZF23" s="0"/>
+      <c r="ZG23" s="0"/>
+      <c r="ZH23" s="0"/>
+      <c r="ZI23" s="0"/>
+      <c r="ZJ23" s="0"/>
+      <c r="ZK23" s="0"/>
+      <c r="ZL23" s="0"/>
+      <c r="ZM23" s="0"/>
+      <c r="ZN23" s="0"/>
+      <c r="ZO23" s="0"/>
+      <c r="ZP23" s="0"/>
+      <c r="ZQ23" s="0"/>
+      <c r="ZR23" s="0"/>
+      <c r="ZS23" s="0"/>
+      <c r="ZT23" s="0"/>
+      <c r="ZU23" s="0"/>
+      <c r="ZV23" s="0"/>
+      <c r="ZW23" s="0"/>
+      <c r="ZX23" s="0"/>
+      <c r="ZY23" s="0"/>
+      <c r="ZZ23" s="0"/>
+      <c r="AAA23" s="0"/>
+      <c r="AAB23" s="0"/>
+      <c r="AAC23" s="0"/>
+      <c r="AAD23" s="0"/>
+      <c r="AAE23" s="0"/>
+      <c r="AAF23" s="0"/>
+      <c r="AAG23" s="0"/>
+      <c r="AAH23" s="0"/>
+      <c r="AAI23" s="0"/>
+      <c r="AAJ23" s="0"/>
+      <c r="AAK23" s="0"/>
+      <c r="AAL23" s="0"/>
+      <c r="AAM23" s="0"/>
+      <c r="AAN23" s="0"/>
+      <c r="AAO23" s="0"/>
+      <c r="AAP23" s="0"/>
+      <c r="AAQ23" s="0"/>
+      <c r="AAR23" s="0"/>
+      <c r="AAS23" s="0"/>
+      <c r="AAT23" s="0"/>
+      <c r="AAU23" s="0"/>
+      <c r="AAV23" s="0"/>
+      <c r="AAW23" s="0"/>
+      <c r="AAX23" s="0"/>
+      <c r="AAY23" s="0"/>
+      <c r="AAZ23" s="0"/>
+      <c r="ABA23" s="0"/>
+      <c r="ABB23" s="0"/>
+      <c r="ABC23" s="0"/>
+      <c r="ABD23" s="0"/>
+      <c r="ABE23" s="0"/>
+      <c r="ABF23" s="0"/>
+      <c r="ABG23" s="0"/>
+      <c r="ABH23" s="0"/>
+      <c r="ABI23" s="0"/>
+      <c r="ABJ23" s="0"/>
+      <c r="ABK23" s="0"/>
+      <c r="ABL23" s="0"/>
+      <c r="ABM23" s="0"/>
+      <c r="ABN23" s="0"/>
+      <c r="ABO23" s="0"/>
+      <c r="ABP23" s="0"/>
+      <c r="ABQ23" s="0"/>
+      <c r="ABR23" s="0"/>
+      <c r="ABS23" s="0"/>
+      <c r="ABT23" s="0"/>
+      <c r="ABU23" s="0"/>
+      <c r="ABV23" s="0"/>
+      <c r="ABW23" s="0"/>
+      <c r="ABX23" s="0"/>
+      <c r="ABY23" s="0"/>
+      <c r="ABZ23" s="0"/>
+      <c r="ACA23" s="0"/>
+      <c r="ACB23" s="0"/>
+      <c r="ACC23" s="0"/>
+      <c r="ACD23" s="0"/>
+      <c r="ACE23" s="0"/>
+      <c r="ACF23" s="0"/>
+      <c r="ACG23" s="0"/>
+      <c r="ACH23" s="0"/>
+      <c r="ACI23" s="0"/>
+      <c r="ACJ23" s="0"/>
+      <c r="ACK23" s="0"/>
+      <c r="ACL23" s="0"/>
+      <c r="ACM23" s="0"/>
+      <c r="ACN23" s="0"/>
+      <c r="ACO23" s="0"/>
+      <c r="ACP23" s="0"/>
+      <c r="ACQ23" s="0"/>
+      <c r="ACR23" s="0"/>
+      <c r="ACS23" s="0"/>
+      <c r="ACT23" s="0"/>
+      <c r="ACU23" s="0"/>
+      <c r="ACV23" s="0"/>
+      <c r="ACW23" s="0"/>
+      <c r="ACX23" s="0"/>
+      <c r="ACY23" s="0"/>
+      <c r="ACZ23" s="0"/>
+      <c r="ADA23" s="0"/>
+      <c r="ADB23" s="0"/>
+      <c r="ADC23" s="0"/>
+      <c r="ADD23" s="0"/>
+      <c r="ADE23" s="0"/>
+      <c r="ADF23" s="0"/>
+      <c r="ADG23" s="0"/>
+      <c r="ADH23" s="0"/>
+      <c r="ADI23" s="0"/>
+      <c r="ADJ23" s="0"/>
+      <c r="ADK23" s="0"/>
+      <c r="ADL23" s="0"/>
+      <c r="ADM23" s="0"/>
+      <c r="ADN23" s="0"/>
+      <c r="ADO23" s="0"/>
+      <c r="ADP23" s="0"/>
+      <c r="ADQ23" s="0"/>
+      <c r="ADR23" s="0"/>
+      <c r="ADS23" s="0"/>
+      <c r="ADT23" s="0"/>
+      <c r="ADU23" s="0"/>
+      <c r="ADV23" s="0"/>
+      <c r="ADW23" s="0"/>
+      <c r="ADX23" s="0"/>
+      <c r="ADY23" s="0"/>
+      <c r="ADZ23" s="0"/>
+      <c r="AEA23" s="0"/>
+      <c r="AEB23" s="0"/>
+      <c r="AEC23" s="0"/>
+      <c r="AED23" s="0"/>
+      <c r="AEE23" s="0"/>
+      <c r="AEF23" s="0"/>
+      <c r="AEG23" s="0"/>
+      <c r="AEH23" s="0"/>
+      <c r="AEI23" s="0"/>
+      <c r="AEJ23" s="0"/>
+      <c r="AEK23" s="0"/>
+      <c r="AEL23" s="0"/>
+      <c r="AEM23" s="0"/>
+      <c r="AEN23" s="0"/>
+      <c r="AEO23" s="0"/>
+      <c r="AEP23" s="0"/>
+      <c r="AEQ23" s="0"/>
+      <c r="AER23" s="0"/>
+      <c r="AES23" s="0"/>
+      <c r="AET23" s="0"/>
+      <c r="AEU23" s="0"/>
+      <c r="AEV23" s="0"/>
+      <c r="AEW23" s="0"/>
+      <c r="AEX23" s="0"/>
+      <c r="AEY23" s="0"/>
+      <c r="AEZ23" s="0"/>
+      <c r="AFA23" s="0"/>
+      <c r="AFB23" s="0"/>
+      <c r="AFC23" s="0"/>
+      <c r="AFD23" s="0"/>
+      <c r="AFE23" s="0"/>
+      <c r="AFF23" s="0"/>
+      <c r="AFG23" s="0"/>
+      <c r="AFH23" s="0"/>
+      <c r="AFI23" s="0"/>
+      <c r="AFJ23" s="0"/>
+      <c r="AFK23" s="0"/>
+      <c r="AFL23" s="0"/>
+      <c r="AFM23" s="0"/>
+      <c r="AFN23" s="0"/>
+      <c r="AFO23" s="0"/>
+      <c r="AFP23" s="0"/>
+      <c r="AFQ23" s="0"/>
+      <c r="AFR23" s="0"/>
+      <c r="AFS23" s="0"/>
+      <c r="AFT23" s="0"/>
+      <c r="AFU23" s="0"/>
+      <c r="AFV23" s="0"/>
+      <c r="AFW23" s="0"/>
+      <c r="AFX23" s="0"/>
+      <c r="AFY23" s="0"/>
+      <c r="AFZ23" s="0"/>
+      <c r="AGA23" s="0"/>
+      <c r="AGB23" s="0"/>
+      <c r="AGC23" s="0"/>
+      <c r="AGD23" s="0"/>
+      <c r="AGE23" s="0"/>
+      <c r="AGF23" s="0"/>
+      <c r="AGG23" s="0"/>
+      <c r="AGH23" s="0"/>
+      <c r="AGI23" s="0"/>
+      <c r="AGJ23" s="0"/>
+      <c r="AGK23" s="0"/>
+      <c r="AGL23" s="0"/>
+      <c r="AGM23" s="0"/>
+      <c r="AGN23" s="0"/>
+      <c r="AGO23" s="0"/>
+      <c r="AGP23" s="0"/>
+      <c r="AGQ23" s="0"/>
+      <c r="AGR23" s="0"/>
+      <c r="AGS23" s="0"/>
+      <c r="AGT23" s="0"/>
+      <c r="AGU23" s="0"/>
+      <c r="AGV23" s="0"/>
+      <c r="AGW23" s="0"/>
+      <c r="AGX23" s="0"/>
+      <c r="AGY23" s="0"/>
+      <c r="AGZ23" s="0"/>
+      <c r="AHA23" s="0"/>
+      <c r="AHB23" s="0"/>
+      <c r="AHC23" s="0"/>
+      <c r="AHD23" s="0"/>
+      <c r="AHE23" s="0"/>
+      <c r="AHF23" s="0"/>
+      <c r="AHG23" s="0"/>
+      <c r="AHH23" s="0"/>
+      <c r="AHI23" s="0"/>
+      <c r="AHJ23" s="0"/>
+      <c r="AHK23" s="0"/>
+      <c r="AHL23" s="0"/>
+      <c r="AHM23" s="0"/>
+      <c r="AHN23" s="0"/>
+      <c r="AHO23" s="0"/>
+      <c r="AHP23" s="0"/>
+      <c r="AHQ23" s="0"/>
+      <c r="AHR23" s="0"/>
+      <c r="AHS23" s="0"/>
+      <c r="AHT23" s="0"/>
+      <c r="AHU23" s="0"/>
+      <c r="AHV23" s="0"/>
+      <c r="AHW23" s="0"/>
+      <c r="AHX23" s="0"/>
+      <c r="AHY23" s="0"/>
+      <c r="AHZ23" s="0"/>
+      <c r="AIA23" s="0"/>
+      <c r="AIB23" s="0"/>
+      <c r="AIC23" s="0"/>
+      <c r="AID23" s="0"/>
+      <c r="AIE23" s="0"/>
+      <c r="AIF23" s="0"/>
+      <c r="AIG23" s="0"/>
+      <c r="AIH23" s="0"/>
+      <c r="AII23" s="0"/>
+      <c r="AIJ23" s="0"/>
+      <c r="AIK23" s="0"/>
+      <c r="AIL23" s="0"/>
+      <c r="AIM23" s="0"/>
+      <c r="AIN23" s="0"/>
+      <c r="AIO23" s="0"/>
+      <c r="AIP23" s="0"/>
+      <c r="AIQ23" s="0"/>
+      <c r="AIR23" s="0"/>
+      <c r="AIS23" s="0"/>
+      <c r="AIT23" s="0"/>
+      <c r="AIU23" s="0"/>
+      <c r="AIV23" s="0"/>
+      <c r="AIW23" s="0"/>
+      <c r="AIX23" s="0"/>
+      <c r="AIY23" s="0"/>
+      <c r="AIZ23" s="0"/>
+      <c r="AJA23" s="0"/>
+      <c r="AJB23" s="0"/>
+      <c r="AJC23" s="0"/>
+      <c r="AJD23" s="0"/>
+      <c r="AJE23" s="0"/>
+      <c r="AJF23" s="0"/>
+      <c r="AJG23" s="0"/>
+      <c r="AJH23" s="0"/>
+      <c r="AJI23" s="0"/>
+      <c r="AJJ23" s="0"/>
+      <c r="AJK23" s="0"/>
+      <c r="AJL23" s="0"/>
+      <c r="AJM23" s="0"/>
+      <c r="AJN23" s="0"/>
+      <c r="AJO23" s="0"/>
+      <c r="AJP23" s="0"/>
+      <c r="AJQ23" s="0"/>
+      <c r="AJR23" s="0"/>
+      <c r="AJS23" s="0"/>
+      <c r="AJT23" s="0"/>
+      <c r="AJU23" s="0"/>
+      <c r="AJV23" s="0"/>
+      <c r="AJW23" s="0"/>
+      <c r="AJX23" s="0"/>
+      <c r="AJY23" s="0"/>
+      <c r="AJZ23" s="0"/>
+      <c r="AKA23" s="0"/>
+      <c r="AKB23" s="0"/>
+      <c r="AKC23" s="0"/>
+      <c r="AKD23" s="0"/>
+      <c r="AKE23" s="0"/>
+      <c r="AKF23" s="0"/>
+      <c r="AKG23" s="0"/>
+      <c r="AKH23" s="0"/>
+      <c r="AKI23" s="0"/>
+      <c r="AKJ23" s="0"/>
+      <c r="AKK23" s="0"/>
+      <c r="AKL23" s="0"/>
+      <c r="AKM23" s="0"/>
+      <c r="AKN23" s="0"/>
+      <c r="AKO23" s="0"/>
+      <c r="AKP23" s="0"/>
+      <c r="AKQ23" s="0"/>
+      <c r="AKR23" s="0"/>
+      <c r="AKS23" s="0"/>
+      <c r="AKT23" s="0"/>
+      <c r="AKU23" s="0"/>
+      <c r="AKV23" s="0"/>
+      <c r="AKW23" s="0"/>
+      <c r="AKX23" s="0"/>
+      <c r="AKY23" s="0"/>
+      <c r="AKZ23" s="0"/>
+      <c r="ALA23" s="0"/>
+      <c r="ALB23" s="0"/>
+      <c r="ALC23" s="0"/>
+      <c r="ALD23" s="0"/>
+      <c r="ALE23" s="0"/>
+      <c r="ALF23" s="0"/>
+      <c r="ALG23" s="0"/>
+      <c r="ALH23" s="0"/>
+      <c r="ALI23" s="0"/>
+      <c r="ALJ23" s="0"/>
+      <c r="ALK23" s="0"/>
+      <c r="ALL23" s="0"/>
+      <c r="ALM23" s="0"/>
+      <c r="ALN23" s="0"/>
+      <c r="ALO23" s="0"/>
+      <c r="ALP23" s="0"/>
+      <c r="ALQ23" s="0"/>
+      <c r="ALR23" s="0"/>
+      <c r="ALS23" s="0"/>
+      <c r="ALT23" s="0"/>
+      <c r="ALU23" s="0"/>
+      <c r="ALV23" s="0"/>
+      <c r="ALW23" s="0"/>
+      <c r="ALX23" s="0"/>
+      <c r="ALY23" s="0"/>
+      <c r="ALZ23" s="0"/>
+      <c r="AMA23" s="0"/>
+      <c r="AMB23" s="0"/>
+      <c r="AMC23" s="0"/>
+      <c r="AMD23" s="0"/>
+      <c r="AME23" s="0"/>
+      <c r="AMF23" s="0"/>
+      <c r="AMG23" s="0"/>
+      <c r="AMH23" s="0"/>
+      <c r="AMI23" s="0"/>
+      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="E24" s="7" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="9" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="J24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="E25" s="7" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="9" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="J25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="E26" s="7" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="9" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="J26" s="10"/>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="1" t="n">
-        <f aca="false">SUM(C7:C26)</f>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <f aca="false">SUM(C7:C27)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12"/>
-      <c r="B36" s="0"/>
+      <c r="B36" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
@@ -4350,22 +4451,33 @@
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
     </row>
-    <row r="37" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="0"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="12"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
     </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="0"/>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4373,8 +4485,8 @@
   <mergeCells count="4">
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="D2:F4"/>
-    <mergeCell ref="A35:J35"/>
-    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="A38:J38"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4398,7 +4510,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.96875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4421,7 +4533,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.96875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Ordered 2-layer PCB from PCBway
</commit_message>
<xml_diff>
--- a/01_Hardware/FlivzNexxy_BOM.xlsx
+++ b/01_Hardware/FlivzNexxy_BOM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="99">
   <si>
     <t xml:space="preserve">xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -209,10 +209,10 @@
     <t xml:space="preserve">C8 </t>
   </si>
   <si>
-    <t xml:space="preserve">CQ0402ARNPO9BNR80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C326068</t>
+    <t xml:space="preserve">CC0402CRNPO9BNR80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C325458</t>
   </si>
   <si>
     <t xml:space="preserve">C9 </t>
@@ -281,10 +281,13 @@
     <t xml:space="preserve">Q2 </t>
   </si>
   <si>
+    <t xml:space="preserve">Born</t>
+  </si>
+  <si>
     <t xml:space="preserve">AO3400A</t>
   </si>
   <si>
-    <t xml:space="preserve">C20917</t>
+    <t xml:space="preserve">C344010</t>
   </si>
   <si>
     <t xml:space="preserve">R1,R2,R4,R8,R9,R14,R15 </t>
@@ -368,10 +371,10 @@
     <t xml:space="preserve">Y1 </t>
   </si>
   <si>
-    <t xml:space="preserve">Abracon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABM3B-32.000MHZ-B2-T</t>
+    <t xml:space="preserve">TXC Corp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7V32000035</t>
   </si>
   <si>
     <t xml:space="preserve">SMD-3225_4P</t>
@@ -691,9 +694,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>665280</xdr:colOff>
+      <xdr:colOff>664560</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -707,7 +710,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="204120"/>
-          <a:ext cx="1352160" cy="374760"/>
+          <a:ext cx="1351440" cy="374040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -730,7 +733,7 @@
   <dimension ref="A2:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+      <selection pane="topLeft" activeCell="E59" activeCellId="0" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1148,10 +1151,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9" t="s">
@@ -1161,7 +1164,7 @@
         <v>15</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J19" s="10"/>
     </row>
@@ -1170,16 +1173,16 @@
         <v>14</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="9" t="s">
@@ -1189,7 +1192,7 @@
         <v>15</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J20" s="10"/>
     </row>
@@ -1198,16 +1201,16 @@
         <v>15</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="9" t="s">
@@ -1217,7 +1220,7 @@
         <v>15</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J21" s="10"/>
       <c r="L21" s="0"/>
@@ -2239,26 +2242,26 @@
         <v>16</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J22" s="10"/>
       <c r="L22" s="0"/>
@@ -3280,26 +3283,26 @@
         <v>17</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J23" s="10"/>
       <c r="L23" s="0"/>
@@ -4321,26 +4324,26 @@
         <v>18</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J24" s="10"/>
     </row>
@@ -4349,26 +4352,26 @@
         <v>19</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H25" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J25" s="10"/>
     </row>
@@ -4377,26 +4380,26 @@
         <v>20</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H26" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J26" s="10"/>
     </row>
@@ -4405,32 +4408,32 @@
         <v>21</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H27" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J27" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C31" s="1" t="n">
         <f aca="false">SUM(C7:C27)</f>
@@ -4440,7 +4443,7 @@
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12"/>
       <c r="B36" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
@@ -4466,7 +4469,7 @@
     <row r="38" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13"/>
       <c r="B38" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
@@ -4510,7 +4513,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.96875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.953125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4533,7 +4536,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.96875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.953125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>